<commit_message>
Add ability to load external files into TPA
</commit_message>
<xml_diff>
--- a/docs/decimal_adjust_accumulator.xlsx
+++ b/docs/decimal_adjust_accumulator.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44005475-6B40-4787-BE6D-B517E9678B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758ED6D7-99CA-4BA3-BC1C-8907164CFC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="768" windowWidth="20076" windowHeight="11472" xr2:uid="{C6E13FBA-B0BB-4402-B9DA-B8D77A4E8680}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -195,7 +195,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,7 +515,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>